<commit_message>
Updated to python 3, cleaned up some awful undergrad code.
</commit_message>
<xml_diff>
--- a/cdc2012_mutations_list.xlsx
+++ b/cdc2012_mutations_list.xlsx
@@ -28,7 +28,7 @@
     <t xml:space="preserve">REFERENCE</t>
   </si>
   <si>
-    <t xml:space="preserve">REF_PROTEIN</t>
+    <t xml:space="preserve">REF_STRAIN</t>
   </si>
   <si>
     <t xml:space="preserve">MUTATION</t>
@@ -701,22 +701,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:J144"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A124" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B147" activeCellId="0" sqref="B147"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B37" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.671875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="91.54"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="23.58"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="25.47"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="5" style="0" width="8.67"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>